<commit_message>
Upload new analysis run
</commit_message>
<xml_diff>
--- a/exports/full_analysis/grafo.xlsx
+++ b/exports/full_analysis/grafo.xlsx
@@ -456,12 +456,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -474,12 +474,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -510,7 +510,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -546,12 +546,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -564,16 +564,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -582,16 +582,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -600,12 +600,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -618,16 +618,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -636,16 +636,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -654,16 +654,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -672,12 +672,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -690,16 +690,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -708,12 +708,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -726,12 +726,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -744,12 +744,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -762,16 +762,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
@@ -780,16 +780,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -798,12 +798,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -816,12 +816,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -834,16 +834,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -852,16 +852,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25">
@@ -870,12 +870,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Energy Transition</t>
+          <t>green transition</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -888,16 +888,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -906,12 +906,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -924,7 +924,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -933,7 +933,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29">
@@ -942,12 +942,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -960,12 +960,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -978,16 +978,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -996,12 +996,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1014,12 +1014,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1032,12 +1032,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1050,16 +1050,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36">
@@ -1068,12 +1068,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1104,12 +1104,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1122,12 +1122,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1140,12 +1140,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1158,12 +1158,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1176,12 +1176,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1194,12 +1194,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1212,12 +1212,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1230,12 +1230,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1248,12 +1248,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1266,16 +1266,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48">
@@ -1284,12 +1284,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Greenhouse Effect</t>
+          <t>greenhouse effect</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1302,16 +1302,16 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1329,7 +1329,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -1338,16 +1338,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -1356,16 +1356,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -1374,12 +1374,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1392,12 +1392,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1410,12 +1410,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1428,16 +1428,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
@@ -1446,16 +1446,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -1464,12 +1464,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1482,12 +1482,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1500,16 +1500,16 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61">
@@ -1518,12 +1518,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1536,12 +1536,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1554,12 +1554,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1572,16 +1572,16 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65">
@@ -1590,12 +1590,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -1644,12 +1644,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -1662,16 +1662,16 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70">
@@ -1680,16 +1680,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>loss of biodiversity</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -1698,7 +1698,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1716,16 +1716,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73">
@@ -1734,12 +1734,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -1752,16 +1752,16 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75">
@@ -1770,12 +1770,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -1788,16 +1788,16 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77">
@@ -1806,16 +1806,16 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78">
@@ -1824,12 +1824,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -1842,12 +1842,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -1860,12 +1860,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -1878,16 +1878,16 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82">
@@ -1896,16 +1896,16 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83">
@@ -1914,12 +1914,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -1932,12 +1932,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -1950,16 +1950,16 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86">
@@ -1968,12 +1968,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -1986,12 +1986,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2004,12 +2004,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2022,12 +2022,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D89" t="n">
@@ -2040,16 +2040,16 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>190</v>
       </c>
     </row>
     <row r="91">
@@ -2058,16 +2058,16 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Extreme weather events</t>
+          <t>extreme weather events</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92">
@@ -2081,11 +2081,11 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93">
@@ -2099,7 +2099,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="D93" t="n">
@@ -2117,11 +2117,11 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -2153,7 +2153,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D97" t="n">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2207,7 +2207,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D100" t="n">
@@ -2243,11 +2243,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D104" t="n">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D105" t="n">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D106" t="n">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D107" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D108" t="n">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D109" t="n">
@@ -2405,11 +2405,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D111" t="n">
@@ -2436,16 +2436,16 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="113">
@@ -2454,16 +2454,16 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114">
@@ -2472,12 +2472,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -2490,12 +2490,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -2508,16 +2508,16 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117">
@@ -2526,16 +2526,16 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118">
@@ -2544,16 +2544,16 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="119">
@@ -2562,12 +2562,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -2580,16 +2580,16 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="121">
@@ -2598,12 +2598,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -2616,12 +2616,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -2634,12 +2634,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -2652,16 +2652,16 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125">
@@ -2670,12 +2670,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -2688,12 +2688,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -2706,12 +2706,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -2724,16 +2724,16 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="129">
@@ -2742,16 +2742,16 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="130">
@@ -2760,12 +2760,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Emissions</t>
+          <t>emissions</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D130" t="n">
@@ -2778,16 +2778,16 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="132">
@@ -2796,12 +2796,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="D132" t="n">
@@ -2814,12 +2814,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -2832,12 +2832,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -2850,16 +2850,16 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136">
@@ -2868,12 +2868,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D136" t="n">
@@ -2886,12 +2886,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -2904,16 +2904,16 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139">
@@ -2922,12 +2922,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -2940,12 +2940,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -2958,12 +2958,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -2976,16 +2976,16 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143">
@@ -2994,12 +2994,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -3012,12 +3012,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -3030,12 +3030,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D145" t="n">
@@ -3048,12 +3048,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D146" t="n">
@@ -3066,16 +3066,16 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="148">
@@ -3084,16 +3084,16 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Global Warming</t>
+          <t>global warming</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="149">
@@ -3102,16 +3102,16 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
@@ -3120,12 +3120,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -3138,16 +3138,16 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="152">
@@ -3156,16 +3156,16 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
@@ -3174,12 +3174,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -3192,12 +3192,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -3210,16 +3210,16 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="156">
@@ -3228,16 +3228,16 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157">
@@ -3246,12 +3246,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -3264,12 +3264,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -3282,16 +3282,16 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="160">
@@ -3300,12 +3300,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -3318,12 +3318,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D161" t="n">
@@ -3336,16 +3336,16 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -3354,12 +3354,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -3372,16 +3372,16 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>108</v>
       </c>
     </row>
     <row r="165">
@@ -3390,16 +3390,16 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Glaciers</t>
+          <t>melting glaciers</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166">
@@ -3408,12 +3408,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -3426,12 +3426,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -3444,16 +3444,16 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="169">
@@ -3462,12 +3462,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D169" t="n">
@@ -3480,12 +3480,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D170" t="n">
@@ -3498,16 +3498,16 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172">
@@ -3516,12 +3516,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -3534,12 +3534,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -3552,12 +3552,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D174" t="n">
@@ -3570,12 +3570,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D175" t="n">
@@ -3588,12 +3588,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -3606,12 +3606,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -3624,12 +3624,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D178" t="n">
@@ -3642,16 +3642,16 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -3660,16 +3660,16 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="181">
@@ -3678,12 +3678,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Renewable Energy</t>
+          <t>renewable energy</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D181" t="n">
@@ -3696,12 +3696,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -3714,12 +3714,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -3732,16 +3732,16 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185">
@@ -3750,12 +3750,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -3768,12 +3768,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -3786,12 +3786,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -3804,12 +3804,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -3822,16 +3822,16 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -3840,12 +3840,12 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -3858,12 +3858,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -3876,12 +3876,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D192" t="n">
@@ -3894,12 +3894,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D193" t="n">
@@ -3912,12 +3912,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D194" t="n">
@@ -3930,16 +3930,16 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196">
@@ -3948,12 +3948,12 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Fake News</t>
+          <t>misinformation</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -3966,16 +3966,16 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198">
@@ -3984,12 +3984,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -4002,12 +4002,12 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -4020,16 +4020,16 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="201">
@@ -4038,12 +4038,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -4056,12 +4056,12 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -4074,12 +4074,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -4092,16 +4092,16 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="205">
@@ -4110,12 +4110,12 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D205" t="n">
@@ -4128,16 +4128,16 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207">
@@ -4146,12 +4146,12 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -4164,12 +4164,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -4182,16 +4182,16 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="210">
@@ -4200,12 +4200,12 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Ecosystem</t>
+          <t>ecosystem</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D210" t="n">
@@ -4218,16 +4218,16 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="212">
@@ -4236,12 +4236,12 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -4254,16 +4254,16 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
@@ -4272,12 +4272,12 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -4290,12 +4290,12 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -4308,12 +4308,12 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -4326,16 +4326,16 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218">
@@ -4344,12 +4344,12 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -4362,12 +4362,12 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -4380,12 +4380,12 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -4398,12 +4398,12 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -4416,16 +4416,16 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="223">
@@ -4434,16 +4434,16 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Fossil Fuels</t>
+          <t>fossil fuels</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="224">
@@ -4452,12 +4452,12 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="D224" t="n">
@@ -4470,12 +4470,12 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D225" t="n">
@@ -4488,12 +4488,12 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -4506,12 +4506,12 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -4524,12 +4524,12 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -4542,16 +4542,16 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="230">
@@ -4560,12 +4560,12 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -4578,12 +4578,12 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -4596,12 +4596,12 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -4614,12 +4614,12 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -4632,16 +4632,16 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>1</v>
+        <v>125</v>
       </c>
     </row>
     <row r="235">
@@ -4650,12 +4650,12 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Energy Consumption</t>
+          <t>energy consumption</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -4668,12 +4668,12 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -4686,12 +4686,12 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -4704,12 +4704,12 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D238" t="n">
@@ -4722,12 +4722,12 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -4740,12 +4740,12 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -4758,12 +4758,12 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -4776,12 +4776,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D242" t="n">
@@ -4794,12 +4794,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -4812,12 +4812,12 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -4830,16 +4830,16 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>0</v>
+        <v>170</v>
       </c>
     </row>
     <row r="246">
@@ -4848,12 +4848,12 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Normatives</t>
+          <t>normatives</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D246" t="n">
@@ -4866,12 +4866,12 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="D247" t="n">
@@ -4884,12 +4884,12 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D248" t="n">
@@ -4902,12 +4902,12 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D249" t="n">
@@ -4920,16 +4920,16 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="251">
@@ -4938,12 +4938,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D251" t="n">
@@ -4956,12 +4956,12 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D252" t="n">
@@ -4974,12 +4974,12 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D253" t="n">
@@ -4992,16 +4992,16 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="255">
@@ -5010,16 +5010,16 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="256">
@@ -5028,16 +5028,16 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Deforestation</t>
+          <t>deforestation</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257">
@@ -5046,12 +5046,12 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="D257" t="n">
@@ -5064,12 +5064,12 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D258" t="n">
@@ -5082,16 +5082,16 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="260">
@@ -5100,12 +5100,12 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -5118,12 +5118,12 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -5136,12 +5136,12 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D262" t="n">
@@ -5154,12 +5154,12 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -5172,16 +5172,16 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="265">
@@ -5190,16 +5190,16 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Flooding</t>
+          <t>flooding</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="266">
@@ -5208,12 +5208,12 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="D266" t="n">
@@ -5226,12 +5226,12 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -5244,12 +5244,12 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -5262,12 +5262,12 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D269" t="n">
@@ -5280,12 +5280,12 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D270" t="n">
@@ -5298,12 +5298,12 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D271" t="n">
@@ -5316,16 +5316,16 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273">
@@ -5334,12 +5334,12 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>tesla</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D273" t="n">
@@ -5352,16 +5352,16 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="275">
@@ -5370,12 +5370,12 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D275" t="n">
@@ -5388,12 +5388,12 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -5406,12 +5406,12 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -5424,12 +5424,12 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D278" t="n">
@@ -5442,16 +5442,16 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="280">
@@ -5460,12 +5460,12 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Green Policies</t>
+          <t>green policies</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D280" t="n">
@@ -5478,12 +5478,12 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="D281" t="n">
@@ -5496,12 +5496,12 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -5514,12 +5514,12 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -5532,12 +5532,12 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -5550,16 +5550,16 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>0</v>
+        <v>254</v>
       </c>
     </row>
     <row r="286">
@@ -5568,12 +5568,12 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Rain</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -5586,12 +5586,12 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="D287" t="n">
@@ -5604,12 +5604,12 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -5622,12 +5622,12 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -5640,16 +5640,16 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="291">
@@ -5658,12 +5658,12 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Electric Vehicles</t>
+          <t>electric vehicles</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -5676,12 +5676,12 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -5694,12 +5694,12 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -5712,16 +5712,16 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>0</v>
+        <v>121</v>
       </c>
     </row>
     <row r="295">
@@ -5730,12 +5730,12 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>natural disaster</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -5748,12 +5748,12 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -5766,16 +5766,16 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="298">
@@ -5784,12 +5784,12 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Clean Energy</t>
+          <t>clean energy</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D298" t="n">
@@ -5802,16 +5802,16 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="300">
@@ -5820,12 +5820,12 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Net Zero</t>
+          <t>net zero</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D300" t="n">
@@ -5838,16 +5838,16 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Tesla</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>Heatwaves</t>
+          <t>heatwaves</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>0</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>